<commit_message>
Add the FrostHeatGrainWt columns for spreadsheets
</commit_message>
<xml_diff>
--- a/Tests/Validation/Canola/Greenethorpe2013.xlsx
+++ b/Tests/Validation/Canola/Greenethorpe2013.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\01-Projects\ApsimX\Tests\Validation\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAD32E0-6BAB-41C8-80BF-3A83274E5090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F718730B-4F69-46DA-95CA-6C42046E94F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$AA$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$AB$29</definedName>
     <definedName name="AvGMCotton">#REF!</definedName>
     <definedName name="AvGMSorg">#REF!</definedName>
     <definedName name="AvGMWht">#REF!</definedName>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
   <si>
     <t>uncut</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>nil</t>
+  </si>
+  <si>
+    <t>Canola.FrostHeatGrainWt</t>
   </si>
 </sst>
 </file>
@@ -198,11 +201,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,44 +519,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7873D758-2B96-4EE8-A7C0-7EBF4418075C}">
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -601,43 +603,46 @@
         <v>22</v>
       </c>
       <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A29" si="0">B2&amp;I2&amp;C2&amp;"Cv"&amp;D2</f>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -660,7 +665,7 @@
       <c r="G2" s="1">
         <v>41401</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2">
         <f>G2-F2</f>
         <v>43</v>
       </c>
@@ -679,14 +684,14 @@
       <c r="N2">
         <v>0</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>1.52</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>169.28</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -709,7 +714,7 @@
       <c r="G3" s="1">
         <v>41444</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3">
         <f t="shared" ref="H3:H29" si="1">G3-F3</f>
         <v>86</v>
       </c>
@@ -728,14 +733,14 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>3.42</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>207.81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -758,7 +763,7 @@
       <c r="G4" s="1">
         <v>41479</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
@@ -777,17 +782,17 @@
       <c r="N4">
         <v>43.252000000000002</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>3.97</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>41</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>182.68</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -810,7 +815,7 @@
       <c r="G5" s="1">
         <v>41492</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <f t="shared" si="1"/>
         <v>134</v>
       </c>
@@ -829,17 +834,17 @@
       <c r="N5">
         <v>107.66500000000001</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>4.4400000000000004</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>43</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>206.06</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -862,7 +867,7 @@
       <c r="G6" s="1">
         <v>41528</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
@@ -881,17 +886,17 @@
       <c r="N6">
         <v>103.479</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>2.96</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>37</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>158.69</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -914,7 +919,7 @@
       <c r="G7" s="1">
         <v>41563</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>205</v>
       </c>
@@ -930,14 +935,14 @@
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
       <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -960,7 +965,7 @@
       <c r="G8" s="1">
         <v>41582</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <f t="shared" si="1"/>
         <v>224</v>
       </c>
@@ -986,28 +991,31 @@
         <v>279.39800000000002</v>
       </c>
       <c r="P8">
+        <v>279.39800000000002</v>
+      </c>
+      <c r="Q8">
         <v>0.28199999999999997</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>4.0250000000000004</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>1360.933</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>69733.97</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>52.042000000000002</v>
       </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
       <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1030,7 +1038,7 @@
       <c r="G9" s="1">
         <v>41470</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
@@ -1041,7 +1049,7 @@
         <v>90.704614800000002</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1064,7 +1072,7 @@
       <c r="G10" s="1">
         <v>41479</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1083,17 +1091,17 @@
       <c r="N10">
         <v>4.734</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>2.15</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>42</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>251.83</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1116,7 +1124,7 @@
       <c r="G11" s="1">
         <v>41485</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1135,17 +1143,17 @@
       <c r="N11">
         <v>3.5129999999999999</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>3.42</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>41</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>302.83999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1168,7 +1176,7 @@
       <c r="G12" s="1">
         <v>41492</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
@@ -1187,17 +1195,17 @@
       <c r="N12">
         <v>8.2449999999999992</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>4.51</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>38</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>286.22000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1220,7 +1228,7 @@
       <c r="G13" s="1">
         <v>41515</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1239,17 +1247,17 @@
       <c r="N13">
         <v>27.68</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>2.75</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>35</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>286.04000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1272,7 +1280,7 @@
       <c r="G14" s="1">
         <v>41570</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -1298,28 +1306,31 @@
         <v>281.60000000000002</v>
       </c>
       <c r="P14">
+        <v>281.60000000000002</v>
+      </c>
+      <c r="Q14">
         <v>0.26300000000000001</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>3.3069999999999999</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>3101.5940000000001</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>85328.501000000004</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>27.488</v>
       </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
       <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1342,7 +1353,7 @@
       <c r="G15" s="1">
         <v>41479</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1361,17 +1372,17 @@
       <c r="N15">
         <v>1.8029999999999999</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>1.6</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>54</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>248.28</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1394,7 +1405,7 @@
       <c r="G16" s="1">
         <v>41479</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1413,17 +1424,17 @@
       <c r="N16">
         <v>2.16</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>1.3</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>41</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>227.21</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1446,7 +1457,7 @@
       <c r="G17" s="1">
         <v>41479</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1465,17 +1476,17 @@
       <c r="N17">
         <v>3.1269999999999998</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>2.37</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>43</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>253.76</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1498,7 +1509,7 @@
       <c r="G18" s="1">
         <v>41485</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1517,23 +1528,23 @@
       <c r="N18">
         <v>4.9390000000000001</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>2.76</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>38</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>295.52</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>6.32</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <v>5.16</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1556,7 +1567,7 @@
       <c r="G19" s="1">
         <v>41485</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1575,23 +1586,23 @@
       <c r="N19">
         <v>3.3239999999999998</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>2.0699999999999998</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>39</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>304.13</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>6.66</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>5.77</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1614,7 +1625,7 @@
       <c r="G20" s="1">
         <v>41485</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1633,23 +1644,23 @@
       <c r="N20">
         <v>5.7629999999999999</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>3.57</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>50</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>306.02999999999997</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>6.53</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <v>5.43</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1672,7 +1683,7 @@
       <c r="G21" s="1">
         <v>41515</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1691,26 +1702,26 @@
       <c r="N21">
         <v>20.265999999999998</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>3.1</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>55</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>282.43</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <v>5.59</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>2.83</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>3.24</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1733,7 +1744,7 @@
       <c r="G22" s="1">
         <v>41515</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1752,26 +1763,26 @@
       <c r="N22">
         <v>19.972000000000001</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>2.23</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>44</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>271.61</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>6.17</v>
       </c>
-      <c r="Y22">
+      <c r="Z22">
         <v>3.82</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <v>3.8</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1794,7 +1805,7 @@
       <c r="G23" s="1">
         <v>41515</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1813,26 +1824,26 @@
       <c r="N23">
         <v>30.544</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>3.15</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>51</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>257.76</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <v>5.54</v>
       </c>
-      <c r="Y23">
+      <c r="Z23">
         <v>2.88</v>
       </c>
-      <c r="AA23">
+      <c r="AB23">
         <v>3.23</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1855,7 +1866,7 @@
       <c r="G24" s="1">
         <v>41543</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
@@ -1874,14 +1885,14 @@
       <c r="N24">
         <v>0</v>
       </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
       <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1904,7 +1915,7 @@
       <c r="G25" s="1">
         <v>41543</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
@@ -1923,14 +1934,14 @@
       <c r="N25">
         <v>0</v>
       </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
       <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1953,7 +1964,7 @@
       <c r="G26" s="1">
         <v>41543</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
@@ -1972,14 +1983,14 @@
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
       <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -2002,7 +2013,7 @@
       <c r="G27" s="1">
         <v>41570</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -2028,31 +2039,34 @@
         <v>335.26600000000002</v>
       </c>
       <c r="P27">
+        <v>335.26600000000002</v>
+      </c>
+      <c r="Q27">
         <v>0.29099999999999998</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>3.1709999999999998</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <v>3084.7750000000001</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>105966.66800000001</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>34.64</v>
       </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
       <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
         <v>41</v>
       </c>
-      <c r="Z27">
+      <c r="AA27">
         <v>1.25</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -2075,7 +2089,7 @@
       <c r="G28" s="1">
         <v>41570</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -2101,31 +2115,34 @@
         <v>209.84899999999999</v>
       </c>
       <c r="P28">
+        <v>209.84899999999999</v>
+      </c>
+      <c r="Q28">
         <v>0.26200000000000001</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>2.79</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <v>2193.924493</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>76401.240489999996</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>35.329523569999999</v>
       </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
       <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
         <v>36</v>
       </c>
-      <c r="Z28">
+      <c r="AA28">
         <v>1.44</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -2148,7 +2165,7 @@
       <c r="G29" s="1">
         <v>41570</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -2174,31 +2191,34 @@
         <v>329.7</v>
       </c>
       <c r="P29">
+        <v>329.7</v>
+      </c>
+      <c r="Q29">
         <v>0.245</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>3.42</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <v>4279.2039999999997</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>95862.459000000003</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>22.439</v>
       </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
       <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
         <v>41</v>
       </c>
-      <c r="Z29">
+      <c r="AA29">
         <v>1.02</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2220,7 +2240,7 @@
       <c r="G41" s="1">
         <v>41563</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41">
         <f t="shared" ref="H41" si="2">G41-F41</f>
         <v>205</v>
       </c>
@@ -2232,7 +2252,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA29" xr:uid="{2557CFD6-CB19-4391-8652-D83569434BCC}"/>
+  <autoFilter ref="A1:AB29" xr:uid="{2557CFD6-CB19-4391-8652-D83569434BCC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>